<commit_message>
uploads and readme updated
</commit_message>
<xml_diff>
--- a/SBI104/SBI104_uploads.xlsx
+++ b/SBI104/SBI104_uploads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Dropbox\Work\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Dropbox\Work\Training\SBI104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{CC7F7D3F-9ABE-47D1-9406-C75758070DDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEEDE07-76E7-4477-940C-ED1464E085F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SBI104" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Competency number</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>DNASequence.docx (third part)</t>
-  </si>
-  <si>
-    <t>INCOMPLETE</t>
   </si>
   <si>
     <t>Questions referring to microbial genomics are in PhylogeneticAnalysis.docx</t>
@@ -150,18 +147,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -372,6 +362,92 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -380,14 +456,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -401,15 +476,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,16 +824,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -762,124 +847,124 @@
       <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="26"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -888,8 +973,8 @@
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>30</v>
+      <c r="D14" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,67 +983,67 @@
       <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>29</v>
+      <c r="D15" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>31</v>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="10"/>
+      <c r="C17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="10"/>
+      <c r="C19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="13"/>
+      <c r="C20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -970,23 +1055,23 @@
       <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="15"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change to suggested uploads
</commit_message>
<xml_diff>
--- a/SBI104/SBI104_uploads.xlsx
+++ b/SBI104/SBI104_uploads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Dropbox\Work\Training\SBI104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saram\Documents\Work\Training\Training\SBI104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEEDE07-76E7-4477-940C-ED1464E085F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E60F9D-70AD-4C9D-A37A-39DE209EC675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SBI104" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Competency number</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Variant interpretation forms from variants analysed in laboratory genetics (clincal cases)</t>
+  </si>
+  <si>
+    <t>Link this competency to the three clinical cases</t>
   </si>
 </sst>
 </file>
@@ -809,21 +812,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
-    <col min="4" max="4" width="68.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" customWidth="1"/>
+    <col min="4" max="4" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -837,7 +840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -849,7 +852,7 @@
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -863,7 +866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="18"/>
       <c r="C4" s="5" t="s">
@@ -873,7 +876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="26"/>
       <c r="B5" s="19"/>
       <c r="C5" s="21" t="s">
@@ -881,7 +884,7 @@
       </c>
       <c r="D5" s="27"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -895,7 +898,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -905,7 +908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -913,7 +916,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -927,7 +930,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -935,7 +938,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -943,7 +946,7 @@
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -951,7 +954,7 @@
       </c>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>5</v>
       </c>
@@ -963,7 +966,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>6</v>
       </c>
@@ -973,105 +976,113 @@
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
         <v>7</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>8</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13" t="s">
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="14"/>
+      <c r="D25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>